<commit_message>
Kfold crossvalidation. 0.833 acc
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>N</t>
   </si>
@@ -177,6 +177,27 @@
   </si>
   <si>
     <t>48 1</t>
+  </si>
+  <si>
+    <t>1 del</t>
+  </si>
+  <si>
+    <t>2 del</t>
+  </si>
+  <si>
+    <t>y+</t>
+  </si>
+  <si>
+    <t>y-</t>
+  </si>
+  <si>
+    <t>y_test</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -505,812 +526,1008 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1">
+      <c r="E2" s="1"/>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-      <c r="K1">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="K2">
+      <c r="L3">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="E4" s="1"/>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="J4">
         <v>11</v>
       </c>
-      <c r="K3">
+      <c r="L4">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>22</v>
+      </c>
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="H4">
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="J5">
         <v>12</v>
       </c>
-      <c r="K4">
+      <c r="L5">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="M5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="E6" s="1"/>
+      <c r="F6">
+        <v>23</v>
+      </c>
+      <c r="G6">
         <v>9</v>
       </c>
-      <c r="H5">
+      <c r="I6">
         <v>41</v>
       </c>
-      <c r="I5">
+      <c r="J6">
         <v>13</v>
       </c>
-      <c r="K5">
+      <c r="L6">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6">
+      <c r="E7" s="1"/>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
         <v>16</v>
       </c>
-      <c r="H6">
+      <c r="I7">
         <v>42</v>
       </c>
-      <c r="I6">
+      <c r="J7">
         <v>14</v>
       </c>
-      <c r="K6">
+      <c r="L7">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7">
+      <c r="E8" s="1"/>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
         <v>17</v>
       </c>
-      <c r="H7">
+      <c r="I8">
         <v>43</v>
       </c>
-      <c r="I7">
+      <c r="J8">
         <v>15</v>
       </c>
-      <c r="K7">
+      <c r="L8">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="M8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
+      <c r="E9" s="1"/>
+      <c r="F9">
+        <v>26</v>
+      </c>
+      <c r="G9">
         <v>18</v>
       </c>
-      <c r="K8">
+      <c r="L9">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="M9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F9">
+      <c r="E10" s="1"/>
+      <c r="F10">
+        <v>27</v>
+      </c>
+      <c r="G10">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10">
+      <c r="E11" s="1"/>
+      <c r="F11">
+        <v>29</v>
+      </c>
+      <c r="G11">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11">
+      <c r="E12" s="1"/>
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12">
+      <c r="E13" s="1"/>
+      <c r="F13">
+        <v>31</v>
+      </c>
+      <c r="G13">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="F17">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="G18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19">
+        <v>47</v>
+      </c>
+      <c r="G19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F19">
+      <c r="E20" s="1"/>
+      <c r="F20">
+        <v>48</v>
+      </c>
+      <c r="G20">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F20">
+      <c r="E21" s="1"/>
+      <c r="F21">
+        <v>52</v>
+      </c>
+      <c r="G21">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F21">
+      <c r="E22" s="1"/>
+      <c r="F22">
+        <v>53</v>
+      </c>
+      <c r="G22">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F22">
+      <c r="E23" s="1"/>
+      <c r="F23">
+        <v>54</v>
+      </c>
+      <c r="G23">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23">
+      <c r="E24" s="1"/>
+      <c r="F24">
+        <v>56</v>
+      </c>
+      <c r="G24">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24">
+      <c r="E25" s="1"/>
+      <c r="F25">
+        <v>57</v>
+      </c>
+      <c r="G25">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F25">
+      <c r="E26" s="1"/>
+      <c r="F26">
+        <v>60</v>
+      </c>
+      <c r="G26">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F26">
+      <c r="E27" s="1"/>
+      <c r="F27">
+        <v>65</v>
+      </c>
+      <c r="G27">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="E28" s="1"/>
+      <c r="F28">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="E29" s="1"/>
+      <c r="F29">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="E30" s="1"/>
+      <c r="F30">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>0</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="E31" s="1"/>
+      <c r="F31">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="E32" s="1"/>
+      <c r="F32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="E33" s="1"/>
+      <c r="F33">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="E34" s="1"/>
+      <c r="F34">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="E35" s="1"/>
+      <c r="F35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="E36" s="1"/>
+      <c r="F36">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="E37" s="1"/>
+      <c r="F37">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="E38" s="1"/>
+      <c r="F38">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="E39" s="1"/>
+      <c r="F39">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>0</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>50</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>51</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>53</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>55</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>56</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>57</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>58</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>59</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>60</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>61</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>62</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1318,7 +1535,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1326,7 +1543,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1334,7 +1551,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1342,7 +1559,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1350,7 +1567,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1358,7 +1575,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1366,7 +1583,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -1374,7 +1591,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1382,7 +1599,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -1390,7 +1607,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -1398,7 +1615,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -1406,7 +1623,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -1414,7 +1631,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -1422,7 +1639,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -1430,7 +1647,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -1438,7 +1655,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -1446,7 +1663,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -1454,7 +1671,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -1462,23 +1679,23 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -1486,7 +1703,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -1494,7 +1711,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -1502,9 +1719,17 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>86</v>
       </c>
-      <c r="B88">
+      <c r="B89">
         <v>1</v>
       </c>
     </row>

</xml_diff>